<commit_message>
Edit Demo 2 Web Results
</commit_message>
<xml_diff>
--- a/4.- Plan de Pruebas/Demo 2 Resultados.xlsx
+++ b/4.- Plan de Pruebas/Demo 2 Resultados.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>Sugerencias (WEB)</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Al añadir un producto a la despensa, que no desaparezca la lista.</t>
   </si>
   <si>
-    <t>Cuando estas añadiendo un producto, que a la derecha se vea la lista de todos los productos de la despensa</t>
-  </si>
-  <si>
     <t>Añadir Producto a la despensa está situado en un sitio que no es intuitivo, una vez que se a pulsado el botón para añadir un producto parece que para añadirlo realmente hay que volver a pulsar.</t>
   </si>
   <si>
@@ -176,13 +173,19 @@
   </si>
   <si>
     <t>Puuuuffffff!!!!!</t>
+  </si>
+  <si>
+    <t>La posición de los botones no se puede cambiar puesto que se desconfiguran otras partes de la web.</t>
+  </si>
+  <si>
+    <t>Cuando estas añadiendo un producto, que a la derecha se vea la lista de todos los productos de la despensa. No se va a hacer puesto que quedaría una lista muy larga de productos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -201,8 +204,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -300,9 +314,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -318,17 +329,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -338,6 +343,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,7 +647,7 @@
   <dimension ref="A1:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -679,38 +690,42 @@
       <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="3" customFormat="1" ht="25.5">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:21" s="3" customFormat="1" ht="38.25">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>11</v>
-      </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="10"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -730,254 +745,288 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="1:21" s="3" customFormat="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:21" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="B9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14" t="s">
+    </row>
+    <row r="10" spans="1:21" s="3" customFormat="1">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:21" s="3" customFormat="1">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:21" s="3" customFormat="1">
+      <c r="A12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:21" s="3" customFormat="1">
+      <c r="A13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:21" s="3" customFormat="1">
+      <c r="A14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:21" s="3" customFormat="1">
+      <c r="A15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:21" s="3" customFormat="1">
+      <c r="A16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="3" customFormat="1">
-      <c r="A10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="16"/>
-    </row>
-    <row r="11" spans="1:21" s="3" customFormat="1">
-      <c r="A11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:21" s="3" customFormat="1">
-      <c r="A12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:21" s="3" customFormat="1">
-      <c r="A13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:21" s="3" customFormat="1">
-      <c r="A14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:21" s="3" customFormat="1">
-      <c r="A15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-    </row>
-    <row r="16" spans="1:21" s="3" customFormat="1">
-      <c r="A16" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A19" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A20" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A22" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A23" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A28" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
+      <c r="C28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" customHeight="1">
       <c r="B29" s="2"/>
@@ -1316,130 +1365,130 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A3" s="18" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A4" s="18" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A5" s="18" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="19" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A7" s="18" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A8" s="18" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="14"/>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A9" s="18" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A10" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A10" s="18" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A11" s="19" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A12" s="19" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A13" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A13" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="9"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="9"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="9"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" s="3" customFormat="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="17"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1809,7 +1858,7 @@
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -1852,40 +1901,40 @@
       <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="3" spans="1:21" s="3" customFormat="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:21" s="3" customFormat="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:21" s="3" customFormat="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1">
       <c r="B7" s="2"/>

</xml_diff>

<commit_message>
Edir Demo 2 Web Results
</commit_message>
<xml_diff>
--- a/4.- Plan de Pruebas/Demo 2 Resultados.xlsx
+++ b/4.- Plan de Pruebas/Demo 2 Resultados.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="54">
   <si>
     <t>Sugerencias (WEB)</t>
   </si>
@@ -292,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -325,9 +325,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -647,7 +644,7 @@
   <dimension ref="A1:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -707,10 +704,10 @@
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="10" t="s">
         <v>53</v>
       </c>
@@ -784,11 +781,11 @@
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="17" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -796,10 +793,10 @@
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
@@ -894,10 +891,10 @@
       <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="12.75" customHeight="1">
@@ -933,17 +930,19 @@
       <c r="B20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="13"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1">
@@ -1010,10 +1009,10 @@
       <c r="A27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" ht="12.75" customHeight="1">
@@ -1365,7 +1364,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="9"/>
@@ -1373,7 +1372,7 @@
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="9"/>
@@ -1381,7 +1380,7 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="9"/>
@@ -1389,7 +1388,7 @@
       <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="9"/>
@@ -1397,7 +1396,7 @@
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="9"/>
@@ -1405,7 +1404,7 @@
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="9"/>
@@ -1413,15 +1412,15 @@
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="14"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="9"/>
@@ -1429,7 +1428,7 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="9"/>
@@ -1437,7 +1436,7 @@
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="9"/>
@@ -1445,7 +1444,7 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="9"/>
@@ -1453,7 +1452,7 @@
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="9"/>
@@ -1488,7 +1487,7 @@
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="14"/>
+      <c r="D18" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1901,13 +1900,13 @@
       <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="6" t="s">
         <v>51</v>
       </c>

</xml_diff>